<commit_message>
update Coachmark SAver & Spender
</commit_message>
<xml_diff>
--- a/DataExcel/TransferNeopay.xlsx
+++ b/DataExcel/TransferNeopay.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nobu\main\Android-Automation\DataExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17FEBE0C-E19F-4042-A149-8A2F2A45103C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F52EA55-46F2-4AA9-A682-F2BFFF03FF14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6427804E-2AB9-E041-9637-7FB925D94670}"/>
   </bookViews>
@@ -34,9 +34,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
   <si>
-    <t>Scenario</t>
-  </si>
-  <si>
     <t>TestType</t>
   </si>
   <si>
@@ -85,7 +82,10 @@
     <t>No Ponsel Tidak terdaftar</t>
   </si>
   <si>
-    <t>Nominal Transfer &gt; max</t>
+    <t>Saldo Kurang</t>
+  </si>
+  <si>
+    <t>Scenario BS+ ke BS</t>
   </si>
 </sst>
 </file>
@@ -449,7 +449,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -462,27 +462,27 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="16.5">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="1">
@@ -491,13 +491,13 @@
     </row>
     <row r="3" spans="1:5" ht="16.5">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D3" s="1">
         <v>50000</v>
@@ -505,13 +505,13 @@
     </row>
     <row r="4" spans="1:5" ht="16.5">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D4" s="1">
         <v>50000</v>
@@ -519,13 +519,13 @@
     </row>
     <row r="5" spans="1:5" ht="16.5">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D5" s="1">
         <v>50000</v>
@@ -533,27 +533,27 @@
     </row>
     <row r="6" spans="1:5" ht="16.5">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D6" s="1">
-        <v>1000000</v>
+        <v>5000000</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="16.5">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D7" s="1">
         <v>50000</v>
@@ -564,13 +564,13 @@
     </row>
     <row r="8" spans="1:5" ht="16.5">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D8" s="1">
         <v>50000</v>

</xml_diff>